<commit_message>
changed tests to simple fcs file
</commit_message>
<xml_diff>
--- a/test/inputs/example.xlsx
+++ b/test/inputs/example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/qr24461_bristol_ac_uk/Documents/Code/eebio-tools/test/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{72607966-65FB-F84D-ABB1-8BAC9771B04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72E8A835-62D2-054D-915D-050491EFAD5A}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{72607966-65FB-F84D-ABB1-8BAC9771B04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B4319A0-9D35-8845-B08C-E205EC3DF92E}"/>
   <bookViews>
-    <workbookView xWindow="19280" yWindow="660" windowWidth="18960" windowHeight="19040" activeTab="3" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
+    <workbookView xWindow="12000" yWindow="1080" windowWidth="18960" windowHeight="17360" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>Plate</t>
   </si>
@@ -81,28 +81,22 @@
     <t>A1</t>
   </si>
   <si>
-    <t>A2</t>
-  </si>
-  <si>
     <t>Flow</t>
   </si>
   <si>
-    <t>/Users/qr24461/OneDrive - University of Bristol/Code/eebio-tools/test/inputs/sample001.fcs</t>
-  </si>
-  <si>
-    <t>/Users/qr24461/OneDrive - University of Bristol/Code/eebio-tools/test/inputs/sample006.fcs</t>
-  </si>
-  <si>
     <t>flow_cy</t>
   </si>
   <si>
     <t>flow_cyt</t>
   </si>
   <si>
-    <t>FSC,SSC,FL1</t>
-  </si>
-  <si>
     <t>process_fcs("plate_01",["FSC","SSC"],["FL1"])</t>
+  </si>
+  <si>
+    <t>/Users/qr24461/OneDrive - University of Bristol/Code/eebio-tools/test/inputs/small.fcs</t>
+  </si>
+  <si>
+    <t>FSC-H,SSC-H,FL1-H,FL1-H,FL3-H,FL1-A,FL4-H</t>
   </si>
 </sst>
 </file>
@@ -485,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2569E313-B3CC-438F-A253-EA0F3E8D819B}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -529,30 +523,13 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -624,7 +601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED90973F-A7AD-4C45-9BA8-61879BED2320}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -643,10 +620,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -674,10 +651,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new esm test data
</commit_message>
<xml_diff>
--- a/test/inputs/example.xlsx
+++ b/test/inputs/example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/qr24461_bristol_ac_uk/Documents/Code/eebio-tools/test/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/qr24461_bristol_ac_uk/Documents/Code/esm/test/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{72607966-65FB-F84D-ABB1-8BAC9771B04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B4319A0-9D35-8845-B08C-E205EC3DF92E}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{72607966-65FB-F84D-ABB1-8BAC9771B04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FAC39769-6F66-5545-8DA2-B0EF68ECBE01}"/>
   <bookViews>
-    <workbookView xWindow="12000" yWindow="1080" windowWidth="18960" windowHeight="17360" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
@@ -90,13 +90,13 @@
     <t>flow_cyt</t>
   </si>
   <si>
-    <t>process_fcs("plate_01",["FSC","SSC"],["FL1"])</t>
-  </si>
-  <si>
     <t>/Users/qr24461/OneDrive - University of Bristol/Code/eebio-tools/test/inputs/small.fcs</t>
   </si>
   <si>
     <t>FSC-H,SSC-H,FL1-H,FL1-H,FL3-H,FL1-A,FL4-H</t>
+  </si>
+  <si>
+    <t>process_fcs("plate_01",["FSC-H","SSC-H"],["FL1-H"])</t>
   </si>
 </sst>
 </file>
@@ -482,7 +482,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -526,10 +526,10 @@
         <v>13</v>
       </c>
       <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
         <v>17</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -575,7 +575,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -602,7 +602,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -623,7 +623,7 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -636,7 +636,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added plate reader tests
testing that plate reader files (read from a directory) are read correctly

small.fcs moved to well 2 in example.xlsx
</commit_message>
<xml_diff>
--- a/test/inputs/example.xlsx
+++ b/test/inputs/example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/qr24461_bristol_ac_uk/Documents/Code/esm/test/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{72607966-65FB-F84D-ABB1-8BAC9771B04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FAC39769-6F66-5545-8DA2-B0EF68ECBE01}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="8_{72607966-65FB-F84D-ABB1-8BAC9771B04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81658FDB-E8D5-424F-86B3-2A4AC9A64612}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
+    <workbookView xWindow="19300" yWindow="680" windowWidth="18960" windowHeight="18940" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>Plate</t>
   </si>
@@ -90,13 +90,37 @@
     <t>flow_cyt</t>
   </si>
   <si>
-    <t>/Users/qr24461/OneDrive - University of Bristol/Code/eebio-tools/test/inputs/small.fcs</t>
+    <t>process_fcs("plate_01",["FSC","SSC"],["FL1"])</t>
   </si>
   <si>
     <t>FSC-H,SSC-H,FL1-H,FL1-H,FL3-H,FL1-A,FL4-H</t>
   </si>
   <si>
-    <t>process_fcs("plate_01",["FSC-H","SSC-H"],["FL1-H"])</t>
+    <t>Plate Reader</t>
+  </si>
+  <si>
+    <t>700,(558,602)</t>
+  </si>
+  <si>
+    <t>558,602</t>
+  </si>
+  <si>
+    <t>700</t>
+  </si>
+  <si>
+    <t>flo</t>
+  </si>
+  <si>
+    <t>OD</t>
+  </si>
+  <si>
+    <t>tecan</t>
+  </si>
+  <si>
+    <t>/Users/qr24461/OneDrive - University of Bristol/Code/esm/test/inputs/small.fcs</t>
+  </si>
+  <si>
+    <t>/Users/qr24461/OneDrive - University of Bristol/Code/esm/test/inputs/pr_folder</t>
   </si>
 </sst>
 </file>
@@ -479,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2569E313-B3CC-438F-A253-EA0F3E8D819B}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -519,16 +543,33 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -543,7 +584,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -560,10 +601,20 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -575,7 +626,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -602,7 +653,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -623,7 +674,7 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -636,7 +687,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated process fcs and example.xlsx for plate 2
fcs file now in plate 2 of example.xlsx
</commit_message>
<xml_diff>
--- a/test/inputs/example.xlsx
+++ b/test/inputs/example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/qr24461_bristol_ac_uk/Documents/Code/esm/test/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="8_{72607966-65FB-F84D-ABB1-8BAC9771B04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81658FDB-E8D5-424F-86B3-2A4AC9A64612}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="8_{72607966-65FB-F84D-ABB1-8BAC9771B04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E21500DC-4E38-9E45-BB84-6D3DE3C074A1}"/>
   <bookViews>
-    <workbookView xWindow="19300" yWindow="680" windowWidth="18960" windowHeight="18940" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
+    <workbookView xWindow="19300" yWindow="620" windowWidth="18960" windowHeight="18940" activeTab="3" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
@@ -90,9 +90,6 @@
     <t>flow_cyt</t>
   </si>
   <si>
-    <t>process_fcs("plate_01",["FSC","SSC"],["FL1"])</t>
-  </si>
-  <si>
     <t>FSC-H,SSC-H,FL1-H,FL1-H,FL3-H,FL1-A,FL4-H</t>
   </si>
   <si>
@@ -121,6 +118,9 @@
   </si>
   <si>
     <t>/Users/qr24461/OneDrive - University of Bristol/Code/esm/test/inputs/pr_folder</t>
+  </si>
+  <si>
+    <t>process_fcs("plate_02",["FSC","SSC"],["FL1"])</t>
   </si>
 </sst>
 </file>
@@ -505,7 +505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2569E313-B3CC-438F-A253-EA0F3E8D819B}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -544,16 +544,16 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" t="s">
-        <v>19</v>
-      </c>
       <c r="G2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -567,10 +567,10 @@
         <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -602,18 +602,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -652,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED90973F-A7AD-4C45-9BA8-61879BED2320}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -674,7 +674,7 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed channel name in transforms example.xlsx
</commit_message>
<xml_diff>
--- a/test/inputs/example.xlsx
+++ b/test/inputs/example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/qr24461_bristol_ac_uk/Documents/Code/esm/test/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="8_{72607966-65FB-F84D-ABB1-8BAC9771B04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E21500DC-4E38-9E45-BB84-6D3DE3C074A1}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="8_{72607966-65FB-F84D-ABB1-8BAC9771B04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0E83BCC-C5D8-E04E-814C-25C064B42FE0}"/>
   <bookViews>
     <workbookView xWindow="19300" yWindow="620" windowWidth="18960" windowHeight="18940" activeTab="3" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
   </bookViews>
@@ -120,7 +120,7 @@
     <t>/Users/qr24461/OneDrive - University of Bristol/Code/esm/test/inputs/pr_folder</t>
   </si>
   <si>
-    <t>process_fcs("plate_02",["FSC","SSC"],["FL1"])</t>
+    <t>process_fcs("plate_02",["FSC-H","SSC-H"],["FL1-H"])</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
example.xlsx now specifies paths through env
filepaths are specified through the environment variable GITHUB_WORKSPACE which allows tests to be run locally or through github actions
</commit_message>
<xml_diff>
--- a/test/inputs/example.xlsx
+++ b/test/inputs/example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/qr24461_bristol_ac_uk/Documents/Code/esm/test/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="8_{72607966-65FB-F84D-ABB1-8BAC9771B04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0E83BCC-C5D8-E04E-814C-25C064B42FE0}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="8_{72607966-65FB-F84D-ABB1-8BAC9771B04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44BA2A2C-2E86-D54C-AA6F-ED95200DE09A}"/>
   <bookViews>
-    <workbookView xWindow="19300" yWindow="620" windowWidth="18960" windowHeight="18940" activeTab="3" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
+    <workbookView xWindow="19300" yWindow="620" windowWidth="18960" windowHeight="18940" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
@@ -114,13 +114,13 @@
     <t>tecan</t>
   </si>
   <si>
-    <t>/Users/qr24461/OneDrive - University of Bristol/Code/esm/test/inputs/small.fcs</t>
-  </si>
-  <si>
-    <t>/Users/qr24461/OneDrive - University of Bristol/Code/esm/test/inputs/pr_folder</t>
-  </si>
-  <si>
     <t>process_fcs("plate_02",["FSC-H","SSC-H"],["FL1-H"])</t>
+  </si>
+  <si>
+    <t>$GITHUB_WORKSPACE/test/inputs/pr_folder</t>
+  </si>
+  <si>
+    <t>$GITHUB_WORKSPACE/test/inputs/small.fcs</t>
   </si>
 </sst>
 </file>
@@ -180,10 +180,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -505,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2569E313-B3CC-438F-A253-EA0F3E8D819B}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -567,7 +563,7 @@
         <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
         <v>16</v>
@@ -652,7 +648,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED90973F-A7AD-4C45-9BA8-61879BED2320}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -674,7 +670,7 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added integration tests for views
</commit_message>
<xml_diff>
--- a/test/inputs/example.xlsx
+++ b/test/inputs/example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qr24461/Library/CloudStorage/OneDrive-UniversityofBristol/Code/esm/test/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712FC0FF-F784-E747-9B33-5B23425B2A11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C18BDF-652D-6D4E-9D12-1637E35511A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11280" yWindow="760" windowWidth="18960" windowHeight="17360" activeTab="4" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
   </bookViews>
@@ -730,7 +730,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -780,7 +780,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated example.xlsx test to use new group format
</commit_message>
<xml_diff>
--- a/test/inputs/example.xlsx
+++ b/test/inputs/example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qr24461/Library/CloudStorage/OneDrive-UniversityofBristol/Code/esm/test/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/qr24461_bristol_ac_uk/Documents/Code/esm/test/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C18BDF-652D-6D4E-9D12-1637E35511A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{19C18BDF-652D-6D4E-9D12-1637E35511A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7261349-D4FB-504E-B830-824E45BA7A2C}"/>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="760" windowWidth="18960" windowHeight="17360" activeTab="4" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
+    <workbookView xWindow="11280" yWindow="760" windowWidth="18960" windowHeight="17360" activeTab="2" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
@@ -129,9 +129,6 @@
     <t>second_group</t>
   </si>
   <si>
-    <t>plate_01_A1,plate_01_A5,plate_01_A9</t>
-  </si>
-  <si>
     <t>third_group</t>
   </si>
   <si>
@@ -162,22 +159,25 @@
     <t>odsub</t>
   </si>
   <si>
-    <t>plate_01_A1,plate_01_A2,plate_01_A3</t>
-  </si>
-  <si>
     <t>hcat(first_group.OD,second_group.OD).-mean(third_group.OD)</t>
   </si>
   <si>
     <t>flowsub</t>
   </si>
   <si>
-    <t>plate_01_A3,plate_01_A8,plate_01_A7</t>
-  </si>
-  <si>
     <t>mega</t>
   </si>
   <si>
     <t>first_group,second_group</t>
+  </si>
+  <si>
+    <t>plate_01_A[1:3]</t>
+  </si>
+  <si>
+    <t>plate_01_A[3,8:-1:7]</t>
+  </si>
+  <si>
+    <t>plate_01_A[1,5,9]</t>
   </si>
 </sst>
 </file>
@@ -678,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D9B2676-373C-45A2-B753-09761E8A63AC}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -700,7 +700,7 @@
         <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -708,15 +708,15 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -756,18 +756,18 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -779,7 +779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80AD15BF-AC00-4821-ADC5-28168A3A0A78}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
@@ -803,7 +803,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
         <v>27</v>
@@ -811,7 +811,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
         <v>28</v>
@@ -819,42 +819,42 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
         <v>37</v>
-      </c>
-      <c r="B6" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove type piracy on mean
introduce new colmean to fix it
update tests to match
</commit_message>
<xml_diff>
--- a/test/inputs/example.xlsx
+++ b/test/inputs/example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/qr24461_bristol_ac_uk/Documents/Code/esm/test/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qr24461/.julia/dev/esm/test/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{19C18BDF-652D-6D4E-9D12-1637E35511A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7261349-D4FB-504E-B830-824E45BA7A2C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D118903-F0E4-E640-A3AA-2BED34058050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="760" windowWidth="18960" windowHeight="17360" activeTab="2" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
+    <workbookView xWindow="11280" yWindow="760" windowWidth="18960" windowHeight="17360" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
@@ -141,9 +141,6 @@
     <t>group3</t>
   </si>
   <si>
-    <t>hcat(first_group.flo,second_group.flo).-mean(third_group.flo)</t>
-  </si>
-  <si>
     <t>flow_sub</t>
   </si>
   <si>
@@ -159,9 +156,6 @@
     <t>odsub</t>
   </si>
   <si>
-    <t>hcat(first_group.OD,second_group.OD).-mean(third_group.OD)</t>
-  </si>
-  <si>
     <t>flowsub</t>
   </si>
   <si>
@@ -178,6 +172,12 @@
   </si>
   <si>
     <t>plate_01_A[1,5,9]</t>
+  </si>
+  <si>
+    <t>hcat(first_group.flo,second_group.flo).-colmean(third_group.flo)</t>
+  </si>
+  <si>
+    <t>hcat(first_group.OD,second_group.OD).-colmean(third_group.OD)</t>
   </si>
 </sst>
 </file>
@@ -558,7 +558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2569E313-B3CC-438F-A253-EA0F3E8D819B}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
@@ -678,7 +678,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D9B2676-373C-45A2-B753-09761E8A63AC}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -700,7 +700,7 @@
         <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -708,7 +708,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -716,7 +716,7 @@
         <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -730,7 +730,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -756,18 +756,18 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -827,34 +827,34 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
         <v>36</v>
-      </c>
-      <c r="B6" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed format name from "tecan" to "generic"
</commit_message>
<xml_diff>
--- a/test/inputs/example.xlsx
+++ b/test/inputs/example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qr24461/.julia/dev/esm/test/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D118903-F0E4-E640-A3AA-2BED34058050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDFEF69D-93CD-0743-8097-E4ECD6EA22D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11280" yWindow="760" windowWidth="18960" windowHeight="17360" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
   </bookViews>
@@ -111,9 +111,6 @@
     <t>OD</t>
   </si>
   <si>
-    <t>tecan</t>
-  </si>
-  <si>
     <t>process_fcs("plate_02",["FSC-H","SSC-H"],["FL1-H"])</t>
   </si>
   <si>
@@ -178,6 +175,9 @@
   </si>
   <si>
     <t>hcat(first_group.OD,second_group.OD).-colmean(third_group.OD)</t>
+  </si>
+  <si>
+    <t>generic</t>
   </si>
 </sst>
 </file>
@@ -559,7 +559,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -600,13 +600,13 @@
         <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
         <v>18</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -620,7 +620,7 @@
         <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
         <v>16</v>
@@ -697,26 +697,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -751,23 +751,23 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -803,58 +803,58 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
         <v>35</v>
-      </c>
-      <c r="B6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
         <v>39</v>
-      </c>
-      <c r="B9" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed example.xlsx to match new template
</commit_message>
<xml_diff>
--- a/test/inputs/example.xlsx
+++ b/test/inputs/example.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qr24461/.julia/dev/esm/test/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{366361CA-585E-9B4B-872F-53BE931ABCDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA38A529-67DE-674A-A184-51589B60F28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="760" windowWidth="18960" windowHeight="17360" activeTab="1" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
+    <workbookView xWindow="19300" yWindow="680" windowWidth="18960" windowHeight="18820" activeTab="4" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
-    <sheet name="ID" sheetId="5" r:id="rId2"/>
+    <sheet name="Channel Map" sheetId="5" r:id="rId2"/>
     <sheet name="Groups" sheetId="2" r:id="rId3"/>
     <sheet name="Transformations" sheetId="3" r:id="rId4"/>
     <sheet name="Views" sheetId="4" r:id="rId5"/>
@@ -51,9 +51,6 @@
     <t>Well</t>
   </si>
   <si>
-    <t>Group</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -66,15 +63,6 @@
     <t>Equation</t>
   </si>
   <si>
-    <t>Groups</t>
-  </si>
-  <si>
-    <t>Current</t>
-  </si>
-  <si>
-    <t>Target</t>
-  </si>
-  <si>
     <t>Plate brand</t>
   </si>
   <si>
@@ -166,6 +154,18 @@
   </si>
   <si>
     <t>OD,flo</t>
+  </si>
+  <si>
+    <t>Channel</t>
+  </si>
+  <si>
+    <t>New name</t>
+  </si>
+  <si>
+    <t>Samples</t>
+  </si>
+  <si>
+    <t>View</t>
   </si>
 </sst>
 </file>
@@ -547,71 +547,71 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="76.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G2" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -624,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA707B9-0BE9-45E5-A5EE-A3873F0594F1}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -635,10 +635,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -657,7 +657,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -670,31 +670,31 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -718,34 +718,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -757,82 +757,82 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80AD15BF-AC00-4821-ADC5-28168A3A0A78}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed process_fcs from tests
</commit_message>
<xml_diff>
--- a/test/inputs/example.xlsx
+++ b/test/inputs/example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qr24461/.julia/dev/esm/test/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA38A529-67DE-674A-A184-51589B60F28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE5AE6B-9C24-D14C-B8BB-52AF14F4FB51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19300" yWindow="680" windowWidth="18960" windowHeight="18820" activeTab="4" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
+    <workbookView xWindow="30380" yWindow="-18700" windowWidth="21280" windowHeight="37580" activeTab="4" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
   <si>
     <t>Plate</t>
   </si>
@@ -72,19 +72,10 @@
     <t>Flow</t>
   </si>
   <si>
-    <t>flow_cy</t>
-  </si>
-  <si>
-    <t>flow_cyt</t>
-  </si>
-  <si>
     <t>FSC-H,SSC-H,FL1-H,FL1-H,FL3-H,FL1-A,FL4-H</t>
   </si>
   <si>
     <t>Plate Reader</t>
-  </si>
-  <si>
-    <t>process_fcs("plate_02",["FSC-H","SSC-H"],["FL1-H"])</t>
   </si>
   <si>
     <t>$GITHUB_WORKSPACE/test/inputs/pr_folder</t>
@@ -582,16 +573,16 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -602,10 +593,10 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -635,10 +626,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -670,31 +661,31 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -705,10 +696,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED90973F-A7AD-4C45-9BA8-61879BED2320}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -726,26 +717,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -755,10 +738,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80AD15BF-AC00-4821-ADC5-28168A3A0A78}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -768,31 +751,31 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -800,7 +783,7 @@
         <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -808,31 +791,23 @@
         <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
         <v>27</v>
-      </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed flow channel format
from FL1-H to FL1_H
</commit_message>
<xml_diff>
--- a/test/inputs/example.xlsx
+++ b/test/inputs/example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qr24461/.julia/dev/esm/test/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE5AE6B-9C24-D14C-B8BB-52AF14F4FB51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E422B4F2-2C9A-AB4D-AD72-F1D17E1D69EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30380" yWindow="-18700" windowWidth="21280" windowHeight="37580" activeTab="4" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19140" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
@@ -72,9 +72,6 @@
     <t>Flow</t>
   </si>
   <si>
-    <t>FSC-H,SSC-H,FL1-H,FL1-H,FL3-H,FL1-A,FL4-H</t>
-  </si>
-  <si>
     <t>Plate Reader</t>
   </si>
   <si>
@@ -157,6 +154,9 @@
   </si>
   <si>
     <t>View</t>
+  </si>
+  <si>
+    <t>FSC_H,SSC_H,FL1_H,FL1_H,FL3_H,FL1_A,FL4_H</t>
   </si>
 </sst>
 </file>
@@ -537,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2569E313-B3CC-438F-A253-EA0F3E8D819B}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -573,16 +573,16 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -593,10 +593,10 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -626,10 +626,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
         <v>35</v>
-      </c>
-      <c r="B1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -661,31 +661,31 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -717,18 +717,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -740,7 +740,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80AD15BF-AC00-4821-ADC5-28168A3A0A78}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -751,63 +751,63 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
         <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
         <v>26</v>
-      </c>
-      <c r="B8" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>